<commit_message>
chore: prepare Win7 build - rounding/sorting/print fixes
</commit_message>
<xml_diff>
--- a/exports/月度统计报表_2025-12.xlsx
+++ b/exports/月度统计报表_2025-12.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="月度统计_2025-12" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="日度统计_2025-12" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -31,29 +31,15 @@
     </font>
     <font>
       <b val="1"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <b val="1"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
       <sz val="12"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00366092"/>
-        <bgColor rgb="00366092"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -68,16 +54,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -443,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,196 +433,241 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>2025-12 月度收费统计报表</t>
+          <t>2025-12 日度收费统计报表</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>统计摘要</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>统计摘要</t>
-        </is>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>总账单数</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>总账单数</t>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>已缴费数</t>
         </is>
       </c>
       <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>未缴费数</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>总金额</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>¥107015.40</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>已缴费金额</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>¥1369.88</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>欠费金额</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>¥105645.52</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>缴费率</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2.2%</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>日期</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>账单数</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>日合计(¥)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>已缴(¥)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>欠费(¥)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-12-16</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
         <v>45</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>已缴费数</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>未缴费数</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>总金额</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>¥107015.40</t>
         </is>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="inlineStr">
-        <is>
-          <t>已缴费金额</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>¥360.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="inlineStr">
-        <is>
-          <t>欠费金额</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>¥106655.40</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="inlineStr">
-        <is>
-          <t>缴费率</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2.2%</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>收费项目明细</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="inlineStr">
-        <is>
-          <t>收费项目</t>
-        </is>
-      </c>
-      <c r="B13" s="4" t="inlineStr">
-        <is>
-          <t>账单数</t>
-        </is>
-      </c>
-      <c r="C13" s="4" t="inlineStr">
-        <is>
-          <t>已缴费数</t>
-        </is>
-      </c>
-      <c r="D13" s="4" t="inlineStr">
-        <is>
-          <t>总金额</t>
-        </is>
-      </c>
-      <c r="E13" s="4" t="inlineStr">
-        <is>
-          <t>已缴费金额</t>
-        </is>
-      </c>
-      <c r="F13" s="4" t="inlineStr">
-        <is>
-          <t>欠费金额</t>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>¥1369.88</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>¥105645.52</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>物业费</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>44</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
+          <t>收费项目</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>账单数</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>已缴费数</t>
+        </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>¥106655.40</t>
+          <t>总金额</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>¥1009.88</t>
+          <t>已缴金额</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>¥105645.52</t>
+          <t>欠费金额</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>生成时间: 2025-12-25 22:20:39</t>
+          <t>物业费</t>
         </is>
       </c>
       <c r="B15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>¥106655.40</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>¥1009.88</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>¥105645.52</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>生成时间: 2025-12-27 12:09:58</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
         <v>1</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C16" t="n">
         <v>1</v>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>¥360.00</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>¥360.00</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>¥0.00</t>
         </is>
@@ -648,7 +675,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Restore full project from D drive for Win7 build
</commit_message>
<xml_diff>
--- a/exports/月度统计报表_2025-12.xlsx
+++ b/exports/月度统计报表_2025-12.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="月度统计_2025-12" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="日度统计_2025-12" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -31,29 +31,15 @@
     </font>
     <font>
       <b val="1"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <b val="1"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
       <sz val="12"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00366092"/>
-        <bgColor rgb="00366092"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -68,16 +54,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -443,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,196 +433,241 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>2025-12 月度收费统计报表</t>
+          <t>2025-12 日度收费统计报表</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>统计摘要</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>统计摘要</t>
-        </is>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>总账单数</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>总账单数</t>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>已缴费数</t>
         </is>
       </c>
       <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>未缴费数</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>总金额</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>¥107015.40</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>已缴费金额</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>¥1369.88</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>欠费金额</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>¥105645.52</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>缴费率</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2.2%</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>日期</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>账单数</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>日合计(¥)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>已缴(¥)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>欠费(¥)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-12-16</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
         <v>45</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>已缴费数</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>未缴费数</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>总金额</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>¥107015.40</t>
         </is>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="inlineStr">
-        <is>
-          <t>已缴费金额</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>¥360.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="inlineStr">
-        <is>
-          <t>欠费金额</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>¥106655.40</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="inlineStr">
-        <is>
-          <t>缴费率</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2.2%</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>收费项目明细</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="inlineStr">
-        <is>
-          <t>收费项目</t>
-        </is>
-      </c>
-      <c r="B13" s="4" t="inlineStr">
-        <is>
-          <t>账单数</t>
-        </is>
-      </c>
-      <c r="C13" s="4" t="inlineStr">
-        <is>
-          <t>已缴费数</t>
-        </is>
-      </c>
-      <c r="D13" s="4" t="inlineStr">
-        <is>
-          <t>总金额</t>
-        </is>
-      </c>
-      <c r="E13" s="4" t="inlineStr">
-        <is>
-          <t>已缴费金额</t>
-        </is>
-      </c>
-      <c r="F13" s="4" t="inlineStr">
-        <is>
-          <t>欠费金额</t>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>¥1369.88</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>¥105645.52</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>物业费</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>44</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
+          <t>收费项目</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>账单数</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>已缴费数</t>
+        </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>¥106655.40</t>
+          <t>总金额</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>¥1009.88</t>
+          <t>已缴金额</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>¥105645.52</t>
+          <t>欠费金额</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>生成时间: 2025-12-25 22:20:39</t>
+          <t>物业费</t>
         </is>
       </c>
       <c r="B15" t="n">
+        <v>44</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>¥106655.40</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>¥1009.88</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>¥105645.52</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>生成时间: 2025-12-27 12:09:58</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
         <v>1</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C16" t="n">
         <v>1</v>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>¥360.00</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>¥360.00</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>¥0.00</t>
         </is>
@@ -648,7 +675,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>